<commit_message>
Captured more metadata for compounds.
SVN: 27085
</commit_message>
<xml_diff>
--- a/openbis-ipad/ipad-example-data/entity-import/samples-materials.xlsx
+++ b/openbis-ipad/ipad-example-data/entity-import/samples-materials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="6080" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="5120" yWindow="6080" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1307">
   <si>
     <t>CODE</t>
   </si>
@@ -2756,6 +2756,1191 @@
   </si>
   <si>
     <t>PROBES</t>
+  </si>
+  <si>
+    <t>FORMULA</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>SMILES</t>
+  </si>
+  <si>
+    <t>C21 H21 N5</t>
+  </si>
+  <si>
+    <t>C=CCN1CCN(CC1)c2nc3ccc4ncccc4c3n5cccc25</t>
+  </si>
+  <si>
+    <t>C20 H18 Cl2 N4 S</t>
+  </si>
+  <si>
+    <t>Clc1ccc(CN2CCN(CC2)c3nc4sccc4n5cccc35)c(Cl)c1</t>
+  </si>
+  <si>
+    <t>C26 H32 N4 O2</t>
+  </si>
+  <si>
+    <t>O=C1N[C@@H](Cc2ccc3[nH]cc(CCN4CC[C@@H](CNCc5ccccc5)C4)c3c2)CO1</t>
+  </si>
+  <si>
+    <t>C27 H29 N O4</t>
+  </si>
+  <si>
+    <t>COc1cccc2OC[C@H](CN3[C@@H]4CC[C@H]3C[C@@](O)(C4)c5ccc6ccccc6c5)Oc12</t>
+  </si>
+  <si>
+    <t>C24 H28 F3 N3 O2</t>
+  </si>
+  <si>
+    <t>CN1C(=O)COc2cc(CCCCN3CCN(CC3)c4cccc(c4)C(F)(F)F)ccc12</t>
+  </si>
+  <si>
+    <t>C10H12ClFN2O2</t>
+  </si>
+  <si>
+    <t>Cl.Oc1cc(F)c(CC2=NCCN2)cc1O</t>
+  </si>
+  <si>
+    <t>C27 H29 F2 N O4</t>
+  </si>
+  <si>
+    <t>Fc1ccc(F)c(CC2CCN(CC2)[C@@H]3CC[C@@]4(CC3)OC(=O)c5c6OCCOc6ccc45)c1</t>
+  </si>
+  <si>
+    <t>C10H11ClN2O2</t>
+  </si>
+  <si>
+    <t>Cl.Oc1ccc(Cc2ncc[nH]2)cc1O</t>
+  </si>
+  <si>
+    <t>C19 H17 Cl N4 S</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1)N2CCN(CC2)c3nc4ccsc4n5cccc35</t>
+  </si>
+  <si>
+    <t>C17 H20 N4 O</t>
+  </si>
+  <si>
+    <t>CN(C)[C@@H]1C[C@H](C1)c2c[nH]c3ccc(cc23)c4onc(C)n4</t>
+  </si>
+  <si>
+    <t>C26 H29 F2 N5</t>
+  </si>
+  <si>
+    <t>Fc1cccc(CCC2(F)CCN(CCCc3c[nH]c4ccc(cc34)n5cnnc5)CC2)c1</t>
+  </si>
+  <si>
+    <t>C28 H36 N6 O</t>
+  </si>
+  <si>
+    <t>CN(Cc1ccccc1C)CC2(O)CCN(CCCc3c[nH]c4ccc(cc34)n5cnnc5)CC2</t>
+  </si>
+  <si>
+    <t>C26 H38 N6 O</t>
+  </si>
+  <si>
+    <t>CC1(C)CCCN(CC2(O)CCN(CCCc3c[nH]c4ccc(cc34)n5cnnc5)CC2)C1</t>
+  </si>
+  <si>
+    <t>C27 H34 N6 O</t>
+  </si>
+  <si>
+    <t>CN(Cc1ccccc1)CC2(O)CCN(CCCc3c[nH]c4ccc(cc34)n5cnnc5)CC2</t>
+  </si>
+  <si>
+    <t>C25 H29 N5</t>
+  </si>
+  <si>
+    <t>C(CN1CCC(Cc2ccccc2)CC1)Cc3c[nH]c4ccc(cc34)n5cnnc5</t>
+  </si>
+  <si>
+    <t>C25 H28 N6 O S</t>
+  </si>
+  <si>
+    <t>CN1CCc2c(C1)sc3N=CN(CCN4CCN(CC4)c5cncc6ccccc56)C(=O)c23</t>
+  </si>
+  <si>
+    <t>C18 H24 N6</t>
+  </si>
+  <si>
+    <t>NC1CCN(CCCc2c[nH]c3ccc(cc23)n4cnnc4)CC1</t>
+  </si>
+  <si>
+    <t>CN1CCN(CCCc2c[nH]c3ccc(cc23)n4cnnc4)CC1</t>
+  </si>
+  <si>
+    <t>C18 H20 N2 O</t>
+  </si>
+  <si>
+    <t>CNCC1CC2N(O1)c3ccccc3Cc4ccccc24</t>
+  </si>
+  <si>
+    <t>C27 H35 N7 O2 S</t>
+  </si>
+  <si>
+    <t>CS(=O)(=O)NC[C@H](NC1CCN(CCCc2c[nH]c3ccc(cc23)n4cnnc4)CC1)c5ccccc5</t>
+  </si>
+  <si>
+    <t>C19 H30 N4 O</t>
+  </si>
+  <si>
+    <t>C(CCNCC1CCc2ccccc2O1)CCNC3=NCCCN3</t>
+  </si>
+  <si>
+    <t>C17 H25 F N4 O</t>
+  </si>
+  <si>
+    <t>Fc1ccc2OC(CNCCCNC3=NCCCN3)CCc2c1</t>
+  </si>
+  <si>
+    <t>C37H46N6O2</t>
+  </si>
+  <si>
+    <t>NC(=O)c1ccc2[nH]cc(C3=CCC(CC3)NCCCCCCCNC4CCC(=CC4)c5c[nH]c6ccc(cc56)C(=O)N)c2c1</t>
+  </si>
+  <si>
+    <t>C18 H25 N O4</t>
+  </si>
+  <si>
+    <t>COC(=O)C1C2CCC(CC1c3ccc(OC)c(OC)c3)N2C</t>
+  </si>
+  <si>
+    <t>C14 H17 N3 O S</t>
+  </si>
+  <si>
+    <t>CN(C)CCO\N=C/1\c2cccn2c3c(C)csc13</t>
+  </si>
+  <si>
+    <t>Cl.Oc1cc(CC2=NCCN2)cc(F)c1O</t>
+  </si>
+  <si>
+    <t>C10H11ClN2O3</t>
+  </si>
+  <si>
+    <t>Cl.OC(c1ccc(O)c(O)c1)c2ncc[nH]2</t>
+  </si>
+  <si>
+    <t>Cl.Oc1ccc(CC2=NCCN2)c(F)c1O</t>
+  </si>
+  <si>
+    <t>C28H35Cl3N4O</t>
+  </si>
+  <si>
+    <t>Cl.CCCn1c(C)c(cc1c2ccccc2)C(=O)NCCCN3CCN(CC3)c4ccc(Cl)c(Cl)c4</t>
+  </si>
+  <si>
+    <t>C31H42N4O</t>
+  </si>
+  <si>
+    <t>CCCn1c(C)c(cc1c2ccccc2)C(=O)N(C)CCCN3CCN(CC3)c4cccc(C)c4C</t>
+  </si>
+  <si>
+    <t>Cl.CCCn1c(C)c(C(=O)NCCN2CCN(CC2)c3cccc(Cl)c3Cl)c(C)c1c4ccccc4</t>
+  </si>
+  <si>
+    <t>C26H31Cl3N4O</t>
+  </si>
+  <si>
+    <t>Cl.Cc1[nH]c(c(C)c1C(=O)NCCCN2CCN(CC2)c3cccc(Cl)c3Cl)c4ccccc4</t>
+  </si>
+  <si>
+    <t>C27H34Cl2N4O</t>
+  </si>
+  <si>
+    <t>Cl.Cc1cccc(N2CCN(CCCNC(=O)c3cc([nH]c3C)c4ccc(Cl)cc4)CC2)c1C</t>
+  </si>
+  <si>
+    <t>C27H34Cl3N5O</t>
+  </si>
+  <si>
+    <t>Cl.CCCn1c(C)c(cc1c2ccccn2)C(=O)NCCCN3CCN(CC3)c4cccc(Cl)c4Cl</t>
+  </si>
+  <si>
+    <t>C26H31FN4O</t>
+  </si>
+  <si>
+    <t>Cc1c(cc(c2ccccc2)n1C)C(=O)NCCCN3CCN(CC3)c4ccc(F)cc4</t>
+  </si>
+  <si>
+    <t>C23H25BrClN5O2</t>
+  </si>
+  <si>
+    <t>Cn1ncc(Br)c1c2cc(NC(=O)Nc3ccc(Cl)cc3)ccc2OCCN4CCCC4</t>
+  </si>
+  <si>
+    <t>C18 H23 F2 N3</t>
+  </si>
+  <si>
+    <t>CC(C)(NC1=NCCNC(=C1)c2ccc(F)cc2F)C3CCC3</t>
+  </si>
+  <si>
+    <t>C23 H28 N4 O</t>
+  </si>
+  <si>
+    <t>CC(C)CN1CCC2(CC1)Oc3ccccc3C4CC(=NN24)c5ccncc5</t>
+  </si>
+  <si>
+    <t>C26H25N3O</t>
+  </si>
+  <si>
+    <t>Cn1c(nc2ccccc12)C3CCN(CC3)C(=O)c4ccc(cc4)c5ccccc5</t>
+  </si>
+  <si>
+    <t>C19H23N3O</t>
+  </si>
+  <si>
+    <t>CCN(CC)C(=O)[C@H]1CN[C@@H]2Cc3c[nH]c4cccc(C2=C1)c34</t>
+  </si>
+  <si>
+    <t>C32H40BrN5O5</t>
+  </si>
+  <si>
+    <t>CC(C)C[C@@H]1N2C(=O)[C@](NC(=O)[C@H]3CN(C)[C@@H]4Cc5c(Br)[nH]c6cccc(C4=C3)c56)(O[C@@]2(O)[C@@H]7CCCN7C1=O)C(C)C</t>
+  </si>
+  <si>
+    <t>C21H24ClN3OS</t>
+  </si>
+  <si>
+    <t>NC(=O)C1CCN(CCCN2c3ccccc3Sc4ccc(Cl)cc24)CC1</t>
+  </si>
+  <si>
+    <t>C23 H26 F N3 O</t>
+  </si>
+  <si>
+    <t>CCCN1CCC2(CC1)Oc3ccccc3C4CC(=NN24)c5ccc(F)cc5</t>
+  </si>
+  <si>
+    <t>C11H16INO2</t>
+  </si>
+  <si>
+    <t>COc1cc(CC(C)N)c(OC)cc1I</t>
+  </si>
+  <si>
+    <t>C20H20N4S</t>
+  </si>
+  <si>
+    <t>C(N1CCN(CC1)c2nc3ccsc3n4cccc24)c5ccccc5</t>
+  </si>
+  <si>
+    <t>C14 H18 N6</t>
+  </si>
+  <si>
+    <t>CN(C)CCc1c[nH]c2ccc(Cn3cnnn3)cc12</t>
+  </si>
+  <si>
+    <t>CN(C)CCc1c[nH]c2ccc(Cc3nn[nH]n3)cc12</t>
+  </si>
+  <si>
+    <t>C21H26F3N3O3S</t>
+  </si>
+  <si>
+    <t>COc1ccc(cc1)S(=O)(=O)NCCCN2CCN(CC2)c3cccc(c3)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>C30H39N3O2S</t>
+  </si>
+  <si>
+    <t>O=S(=O)(N(CCCN1CCN(CC1)c2ccccc2)CC3CCCCC3)c4ccc5ccccc5c4</t>
+  </si>
+  <si>
+    <t>C29H36Cl2N4O2S</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1Cl)N2CCN(CCCN(CC3CCCCC3)S(=O)(=O)c4cccc5cccnc45)CC2</t>
+  </si>
+  <si>
+    <t>Clc1ccc(CN2CCN(CC2)c3nc4sccc4n5cccc35)cc1Cl</t>
+  </si>
+  <si>
+    <t>C16 H19 N3 O S</t>
+  </si>
+  <si>
+    <t>Cc1csc2\C(=N/OCCN3CCCC3)\c4cccn4c12</t>
+  </si>
+  <si>
+    <t>C22 H21 F N4</t>
+  </si>
+  <si>
+    <t>Fc1ccc(CN2CCN(CC2)c3nc4ccccc4n5cccc35)cc1</t>
+  </si>
+  <si>
+    <t>C26H30N6O</t>
+  </si>
+  <si>
+    <t>Cc1cccc2C(=O)N(N)C(=Nc12)CCCCN3CCN(CC3)c4ccc5ccccc5n4</t>
+  </si>
+  <si>
+    <t>C21 H23 N3 O S</t>
+  </si>
+  <si>
+    <t>CN(CCCO\N=C/1\c2cccn2c3c(C)csc13)Cc4ccccc4</t>
+  </si>
+  <si>
+    <t>C15 H16 Cl N3 O</t>
+  </si>
+  <si>
+    <t>CN(C)CCO\N=C\1/c2cc(Cl)ccc2n3cccc13</t>
+  </si>
+  <si>
+    <t>C19 H20 F2 N2 O</t>
+  </si>
+  <si>
+    <t>CN(C)CC1CC2N(O1)c3cc(F)ccc3Cc4ccc(F)cc24</t>
+  </si>
+  <si>
+    <t>C41 H47 N4 O2 . Br</t>
+  </si>
+  <si>
+    <t>[Br-].C=CC[N+]12CC[C@H]3[C@@H]1C[C@@H]4[C@H]5[C@@H](OCC=C4C2)N6[C@H]7[C@H]8[C@H]9C[C@@H]%10N(CC[C@]7%10c%11ccccc6%11)CC9=CCO[C@H]8N([C@H]35)c%12ccccc%12</t>
+  </si>
+  <si>
+    <t>C22 H23 N5 O</t>
+  </si>
+  <si>
+    <t>COc1ccc2nc(N3CCN(Cc4ccccc4)CC3)c5cccn5c2n1</t>
+  </si>
+  <si>
+    <t>C38 H42 N4 O2</t>
+  </si>
+  <si>
+    <t>C1CN2CC3=CCO[C@@H]4[C@@H]5[C@H]3C[C@H]2[C@H]1[C@H]5N([C@@H]6OCC=C7CN8CC[C@@]9%10[C@@H]8C[C@@H]7[C@@H]6[C@@H]9N4c%11ccccc%10%11)c%12ccccc%12</t>
+  </si>
+  <si>
+    <t>C18H20N2</t>
+  </si>
+  <si>
+    <t>CN1CCN2C(C1)c3ccccc3Cc4ccccc24</t>
+  </si>
+  <si>
+    <t>C13 H15 N3 O S</t>
+  </si>
+  <si>
+    <t>CN(C)CCO\N=C/1\c2cccn2c3ccsc13</t>
+  </si>
+  <si>
+    <t>C15 H17 N3 O</t>
+  </si>
+  <si>
+    <t>CN(C)CCO\N=C\1/c2ccccc2n3cccc13</t>
+  </si>
+  <si>
+    <t>C15H19N5</t>
+  </si>
+  <si>
+    <t>CN(C)CCc1c[nH]c2ccc(Cn3cncn3)cc12</t>
+  </si>
+  <si>
+    <t>C17 H25 Cl N2 O3</t>
+  </si>
+  <si>
+    <t>COc1cc(N)c(Cl)cc1C(=O)OCCN2CC(C)CC(C)C2</t>
+  </si>
+  <si>
+    <t>C21 H29 N3 O2</t>
+  </si>
+  <si>
+    <t>CCCCN1CCC(CNC(=O)c2c3OCCn3c4ccccc24)CC1</t>
+  </si>
+  <si>
+    <t>C14H20ClN3O3</t>
+  </si>
+  <si>
+    <t>COC1CNCCC1NC(=O)c2cc(Cl)c(N)cc2OC</t>
+  </si>
+  <si>
+    <t>C23 H38 Cl N5 O2</t>
+  </si>
+  <si>
+    <t>COc1cc(N)c(Cl)cc1C(=O)NC2CCN(CC3CCN(CCCCN)CC3)CC2</t>
+  </si>
+  <si>
+    <t>C14H21ClN2O3</t>
+  </si>
+  <si>
+    <t>CCN(CC)CCOC(=O)c1cc(Cl)c(N)cc1OC</t>
+  </si>
+  <si>
+    <t>C21 H32 Cl N5 O3</t>
+  </si>
+  <si>
+    <t>COc1cc(N)c(Cl)cc1C(=O)NC2CCN(CC3CCN(CC3)C(=O)CN)CC2</t>
+  </si>
+  <si>
+    <t>C17 H26 N4 O2 S</t>
+  </si>
+  <si>
+    <t>CN(C)CCc1c[nH]c2ccc(CN3CC(C)(C)NS3(=O)=O)cc12</t>
+  </si>
+  <si>
+    <t>C16 H24 N4 O2 S</t>
+  </si>
+  <si>
+    <t>CN(C)CCc1c[nH]c2ccc(CCN3CCNS3(=O)=O)cc12</t>
+  </si>
+  <si>
+    <t>C14H21N3O2S</t>
+  </si>
+  <si>
+    <t>CNS(=O)(=O)Cc1ccc2[nH]cc(CCN(C)C)c2c1</t>
+  </si>
+  <si>
+    <t>C22 H22 N2 O2 S</t>
+  </si>
+  <si>
+    <t>CN(C)CCn1cc(c2ccccc12)S(=O)(=O)c3cccc4ccccc34</t>
+  </si>
+  <si>
+    <t>C21H22F3N3O2S</t>
+  </si>
+  <si>
+    <t>CN1CCC[C@H]1Cc2c[nH]c3ccc(NS(=O)(=O)c4ccc(cc4)C(F)(F)F)cc23</t>
+  </si>
+  <si>
+    <t>C19 H19 I N2 O2 S</t>
+  </si>
+  <si>
+    <t>CN1CCC(C1)c2cn(c3ccccc23)S(=O)(=O)c4ccc(I)cc4</t>
+  </si>
+  <si>
+    <t>C22H21ClN4O2S</t>
+  </si>
+  <si>
+    <t>NC1CCN(CC1)c2ccc3[nH]nc(c3c2)S(=O)(=O)c4cccc5c(Cl)cccc45</t>
+  </si>
+  <si>
+    <t>C18H19ClN4O2S</t>
+  </si>
+  <si>
+    <t>NC1CCN(CC1)c2ccc3[nH]nc(c3c2)S(=O)(=O)c4cccc(Cl)c4</t>
+  </si>
+  <si>
+    <t>C23H24N4O2S</t>
+  </si>
+  <si>
+    <t>CN1CCN(CC1)c2ccc3c(c2)c(nn3C)S(=O)(=O)c4cccc5ccccc45</t>
+  </si>
+  <si>
+    <t>C23H23ClN4O3S</t>
+  </si>
+  <si>
+    <t>Cl.O=C(Nc1cccc2c(n[nH]c12)S(=O)(=O)c3cccc4ccccc34)C5CCCNC5</t>
+  </si>
+  <si>
+    <t>C30H33N5O2</t>
+  </si>
+  <si>
+    <t>Cc1cccc(N2CCN(CCC(=O)NCC3=Nc4ccccc4C(=O)N3c5ccccc5)CC2)c1C</t>
+  </si>
+  <si>
+    <t>C30H32FN5O2</t>
+  </si>
+  <si>
+    <t>Cc1ccc(N2CCN(CCC(=O)NCC3=Nc4ccccc4C(=O)N3c5ccc(F)cc5)CC2)c(C)c1</t>
+  </si>
+  <si>
+    <t>C31H34FN5O2</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1C)N2CCN(CCCC(=O)NCC3=Nc4ccc(F)cc4C(=O)N3c5ccccc5)CC2</t>
+  </si>
+  <si>
+    <t>C29H31N5O3</t>
+  </si>
+  <si>
+    <t>COc1ccccc1N2CCN(CCC(=O)NCC3=Nc4ccccc4C(=O)N3c5ccccc5)CC2</t>
+  </si>
+  <si>
+    <t>C17H21N3OS</t>
+  </si>
+  <si>
+    <t>CCN1CCC(COc2nc3ccsc3n4cccc24)CC1</t>
+  </si>
+  <si>
+    <t>C23 H25 Br F3 N5 O3 S</t>
+  </si>
+  <si>
+    <t>CN(C)c1nc(NCC2CCN(CC2)S(=O)(=O)c3ccc(Br)cc3OC(F)(F)F)nc4ccccc14</t>
+  </si>
+  <si>
+    <t>C18 H21 N3 O</t>
+  </si>
+  <si>
+    <t>CN(C)CC1CC2N(O1)c3cnccc3Cc4ccccc24</t>
+  </si>
+  <si>
+    <t>C23 H23 N3 O2</t>
+  </si>
+  <si>
+    <t>CC1=CN2C(=O)C(=C(C)N=C2C=C1)CCN3CCc4oc5ccccc5c4C3</t>
+  </si>
+  <si>
+    <t>C20 H24 N2 O</t>
+  </si>
+  <si>
+    <t>CN(C)CCC1CC2N(O1)c3ccccc3Cc4ccccc24</t>
+  </si>
+  <si>
+    <t>C15H15ClN2</t>
+  </si>
+  <si>
+    <t>Cl.CC(c1c[nH]cn1)c2cccc3ccccc23</t>
+  </si>
+  <si>
+    <t>C26 H29 Br F3 N5 O2</t>
+  </si>
+  <si>
+    <t>CN(C)c1nc(NCC2CCC(CNC(=O)c3ccc(Br)cc3OC(F)(F)F)CC2)nc4ccccc14</t>
+  </si>
+  <si>
+    <t>C22 H21 N3 O3</t>
+  </si>
+  <si>
+    <t>CC1=C(CCN2CCc3oc4ccccc4c3C2)C(=O)N5C=CC=C(O)C5=N1</t>
+  </si>
+  <si>
+    <t>CC1=CC2=NC(=C(CCN3CCc4oc5ccccc5c4C3)C(=O)N2C=C1)C</t>
+  </si>
+  <si>
+    <t>C24H26N2O4</t>
+  </si>
+  <si>
+    <t>COc1ccccc1OCCNCC(O)COc2cccc3[nH]c4ccccc4c23</t>
+  </si>
+  <si>
+    <t>C47H80O17</t>
+  </si>
+  <si>
+    <t>CO[C@H]1C[C@@H](O[C@H]2C[C@@H](O[C@H]2[C@]3(C)CC[C@@H](O3)[C@]4(C)CC[C@]5(C[C@H](O)[C@@H](C)[C@H](O5)[C@@H](C)[C@@H]6O[C@](O)(CC(=O)O)[C@@H](C)[C@H](OC)[C@H]6OC)O4)[C@H]7O[C@](C)(O)[C@H](C)C[C@@H]7C)O[C@@H](C)[C@@H]1OC</t>
+  </si>
+  <si>
+    <t>C20H23N</t>
+  </si>
+  <si>
+    <t>CN(C)CCC=C1c2ccccc2CCc3ccccc13</t>
+  </si>
+  <si>
+    <t>Cl.CC(c1cccc2ccccc12)c3ncc[nH]3</t>
+  </si>
+  <si>
+    <t>C21H26N2O3</t>
+  </si>
+  <si>
+    <t>COC(=O)[C@H]1[C@@H](O)CC[C@H]2CN3CCc4c([nH]c5ccccc45)[C@@H]3C[C@H]12</t>
+  </si>
+  <si>
+    <t>C22H26F3N3OS</t>
+  </si>
+  <si>
+    <t>OCCN1CCN(CCCN2c3ccccc3Sc4ccc(cc24)C(F)(F)F)CC1</t>
+  </si>
+  <si>
+    <t>C28H37NO4</t>
+  </si>
+  <si>
+    <t>COCCOc1cc2CC[C@@H]3[C@H](CC[C@@]4(C)[C@H]3CC[C@@]45CCC(C)(C)C(=O)O5)c2cc1C#N</t>
+  </si>
+  <si>
+    <t>C23H30O3</t>
+  </si>
+  <si>
+    <t>C[C@]12CC[C@H]3[C@@H](CCc4cc(O)ccc34)[C@@H]1CC[C@@]25CCCCC(=O)O5</t>
+  </si>
+  <si>
+    <t>CC1CC[C@@]2(CC[C@H]3[C@@H]4CCc5cc(O)ccc5[C@H]4CC[C@]23C)OC1=O</t>
+  </si>
+  <si>
+    <t>C24H32O2</t>
+  </si>
+  <si>
+    <t>CC1(C)CC[C@@]2(CC[C@H]3[C@@H]4CCc5ccccc5[C@H]4CC[C@]23C)OC1=O</t>
+  </si>
+  <si>
+    <t>C23H30O2</t>
+  </si>
+  <si>
+    <t>CC1CC[C@@]2(CC[C@H]3[C@@H]4CCc5ccccc5[C@H]4CC[C@]23C)OC1=O</t>
+  </si>
+  <si>
+    <t>C13H10N2O4</t>
+  </si>
+  <si>
+    <t>OC(=O)c1cccc(Nc2ccc(cc2)[N+](=O)[O-])c1</t>
+  </si>
+  <si>
+    <t>C15H13NO3</t>
+  </si>
+  <si>
+    <t>CC(=O)c1ccc(Nc2cccc(c2)C(=O)O)cc1</t>
+  </si>
+  <si>
+    <t>CC1CC(=O)O[C@]2(CC[C@H]3[C@@H]4CCc5cc(O)ccc5[C@H]4CC[C@]23C)C1</t>
+  </si>
+  <si>
+    <t>C22H26O3</t>
+  </si>
+  <si>
+    <t>C[C@]12CC[C@H]3[C@@H](CCc4cc(O)ccc34)[C@@H]1CC[C@@]25CC=CC(=O)O5</t>
+  </si>
+  <si>
+    <t>C22H28O2</t>
+  </si>
+  <si>
+    <t>C[C@]12CC[C@H]3[C@@H](CCc4ccccc34)[C@@H]1CC[C@@]25CCCC(=O)O5</t>
+  </si>
+  <si>
+    <t>C25H33NO3</t>
+  </si>
+  <si>
+    <t>CC1(C)CC[C@@]2(CC[C@H]3[C@@H]4CCc5cc(ccc5[C@H]4CC[C@]23C)C(=O)N)OC1=O</t>
+  </si>
+  <si>
+    <t>C16H17F2N3S</t>
+  </si>
+  <si>
+    <t>C[C@@H]1CCCC/C/1=N/Nc2nc(cs2)c3ccc(F)cc3F</t>
+  </si>
+  <si>
+    <t>C14 H15 N3 S</t>
+  </si>
+  <si>
+    <t>C1CCC(=NNc2nc(cs2)c3ccccc3)C1</t>
+  </si>
+  <si>
+    <t>C11 H8 O3</t>
+  </si>
+  <si>
+    <t>OC(=O)C1=Cc2ccccc2CC1=O</t>
+  </si>
+  <si>
+    <t>C16H18N4O2S</t>
+  </si>
+  <si>
+    <t>C[C@@H]1CCCC/C/1=N\Nc2nc(cs2)c3ccc(cc3)[N+](=O)[O-]</t>
+  </si>
+  <si>
+    <t>C26H26N4O3</t>
+  </si>
+  <si>
+    <t>COc1cc(cc(OC)c1OC)\C(=N\Nc2nc3ccccc3nc2Cc4ccccc4)\C</t>
+  </si>
+  <si>
+    <t>C24H18BrN5O</t>
+  </si>
+  <si>
+    <t>CN(C)c1ccc(cc1Br)c2nnc3c(nc4ccccc4n23)C(=O)c5ccccc5</t>
+  </si>
+  <si>
+    <t>C11 H7 Br O3</t>
+  </si>
+  <si>
+    <t>OC(=O)C1=Cc2cc(Br)ccc2CC1=O</t>
+  </si>
+  <si>
+    <t>C19 H20 N2 O4</t>
+  </si>
+  <si>
+    <t>COc1ccc(C2CC(=NN2C(=O)C)c3ccc(O)cc3)c(OC)c1</t>
+  </si>
+  <si>
+    <t>C19 H18 O5</t>
+  </si>
+  <si>
+    <t>CC1=Cc2ccc(OC\C=C\C3=CC(=O)C(C)(C)O3)cc2OC1=O</t>
+  </si>
+  <si>
+    <t>C16H11BrO3</t>
+  </si>
+  <si>
+    <t>Brc1ccc(COc2ccc3OC=CC(=O)c3c2)cc1</t>
+  </si>
+  <si>
+    <t>COc1ccc(cc1)c2csc(NN=C3CCCCCC3)n2</t>
+  </si>
+  <si>
+    <t>C21 H22 O5</t>
+  </si>
+  <si>
+    <t>C\C(=C/COc1ccc2C(=C(C)C(=O)Oc2c1)C)\C3=CC(=O)C(C)(C)O3</t>
+  </si>
+  <si>
+    <t>C18 H15 N3 O2 S</t>
+  </si>
+  <si>
+    <t>S=C1OC(=NN1CCC#N)c2ccc(OCc3ccccc3)cc2</t>
+  </si>
+  <si>
+    <t>C16H10FNO3</t>
+  </si>
+  <si>
+    <t>Fc1ccc(NC(=O)C2=Cc3ccccc3OC2=O)cc1</t>
+  </si>
+  <si>
+    <t>C15H15Cl2N3S</t>
+  </si>
+  <si>
+    <t>Clc1ccc(c(Cl)c1)c2csc(NN=C3CCCCC3)n2</t>
+  </si>
+  <si>
+    <t>C17 H9 F N2 O</t>
+  </si>
+  <si>
+    <t>Fc1cccc(c1)c2cc3C(=O)c4ccccc4c3nn2</t>
+  </si>
+  <si>
+    <t>C18 H15 N3 O3</t>
+  </si>
+  <si>
+    <t>O=C1OC(=NN1CCC#N)c2ccc(OCc3ccccc3)cc2</t>
+  </si>
+  <si>
+    <t>C12H13N</t>
+  </si>
+  <si>
+    <t>C#CCN[C@H]1CCc2ccccc12</t>
+  </si>
+  <si>
+    <t>C16H13F3N4OS</t>
+  </si>
+  <si>
+    <t>Cc1cc(Nc2nccc(n2)c3nc(CO)cs3)cc(c1)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>C14H18N6O</t>
+  </si>
+  <si>
+    <t>Cc1cccc(Nc2nc(NCCN)ncc2C(=O)N)c1</t>
+  </si>
+  <si>
+    <t>C14H17N5O2</t>
+  </si>
+  <si>
+    <t>Cc1cccc(Nc2nc(OCCN)ncc2C(=O)N)c1</t>
+  </si>
+  <si>
+    <t>C16H20N6O</t>
+  </si>
+  <si>
+    <t>Cc1cccc(Nc2nc(N[C@@H]3CCNC3)ncc2C(=O)N)c1</t>
+  </si>
+  <si>
+    <t>C17H22N6O2</t>
+  </si>
+  <si>
+    <t>Cc1cccc(Nc2nc(N[C@@H]3CCOC[C@@H]3N)ncc2C(=O)N)c1</t>
+  </si>
+  <si>
+    <t>C18H22F2N6O</t>
+  </si>
+  <si>
+    <t>Cc1cccc(Nc2nc(N[C@@H]3CC(F)(F)CC[C@@H]3N)ncc2C(=O)N)c1</t>
+  </si>
+  <si>
+    <t>C18H15N3O3S</t>
+  </si>
+  <si>
+    <t>Cn1cc(\C=C\2/C(=O)Nc3ccc(cc23)S(=O)(=O)N)c4ccccc14</t>
+  </si>
+  <si>
+    <t>C22H22N4O5S</t>
+  </si>
+  <si>
+    <t>COc1ccc2c(c1)c(\C=C\3/C(=O)Nc4ccc(cc34)S(=O)(=O)NCCC(=O)N)cn2C</t>
+  </si>
+  <si>
+    <t>C26 H21 N3 O6 S</t>
+  </si>
+  <si>
+    <t>COc1ccc2c(c1)c(\C=C\3/C(=O)Nc4ccc(cc34)S(=O)(=O)N)cn2Cc5cccc(c5)C(=O)O</t>
+  </si>
+  <si>
+    <t>C28 H26 N4 O3</t>
+  </si>
+  <si>
+    <t>CN[C@@H]1CC2O[C@@](C)([C@@H]1OC)n3c4ccccc4c5c6CNC(=O)c6c7c8ccccc8n2c7c35</t>
+  </si>
+  <si>
+    <t>C18H20N4</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)c2cc3ncccc3c(NCCCN)n2</t>
+  </si>
+  <si>
+    <t>C11 H10 N2 O3</t>
+  </si>
+  <si>
+    <t>Cc1cc(C)c2c(O)c(N=O)c(O)nc2c1</t>
+  </si>
+  <si>
+    <t>C9 H6 Cl N3 O4</t>
+  </si>
+  <si>
+    <t>Cc1cc2nc(O)c(O)nc2c(c1Cl)[N+](=O)[O-]</t>
+  </si>
+  <si>
+    <t>C21 H22 N2 O2</t>
+  </si>
+  <si>
+    <t>Oc1cccc2[nH]c(cc12)C(=O)N3CCC(Cc4ccccc4)CC3</t>
+  </si>
+  <si>
+    <t>C87H141N27O33</t>
+  </si>
+  <si>
+    <t>CC[C@H](C)[C@H](NC(=O)[C@H](CC(C)C)NC(=O)[C@H](CCC(=O)O)NC(=O)[C@H](CCC(=O)N)NC(=O)[C@H](CC(=O)N)NC(=O)[C@H](CCCCN)NC(=O)[C@H](CCC(=O)N)NC(=O)[C@H](Cc1ccc(O)cc1)NC(=O)[C@H](CCC(=O)O)NC(=O)[C@H](CCC(=O)O)NC(=O)[C@H](CCC(=O)O)NC(=O)CN)C(=O)N[C@@H](CCCN=C(N)N)C(=O)N[C@@H](CCC(=O)O)C(=O)N[C@@H](CCCCN)C(=O)N[C@@H](CO)C(=O)N[C@@H](CC(=O)N)C(=O)N</t>
+  </si>
+  <si>
+    <t>C9 H6 Br N3 O5</t>
+  </si>
+  <si>
+    <t>COc1c(Br)cc2nc(O)c(O)nc2c1[N+](=O)[O-]</t>
+  </si>
+  <si>
+    <t>C21 H22 N2 O3</t>
+  </si>
+  <si>
+    <t>Oc1cc(O)c2cc([nH]c2c1)C(=O)N3CCC(Cc4ccccc4)CC3</t>
+  </si>
+  <si>
+    <t>C10 H8 Cl N3 O4</t>
+  </si>
+  <si>
+    <t>CCc1cc2nc(O)c(O)nc2c(c1Cl)[N+](=O)[O-]</t>
+  </si>
+  <si>
+    <t>C23 H25 N3 O4</t>
+  </si>
+  <si>
+    <t>Cc1ccc(CC2CCN(CC2)C(=O)C(=O)Nc3ccc4NC(=O)COc4c3)cc1</t>
+  </si>
+  <si>
+    <t>C22H29NO2</t>
+  </si>
+  <si>
+    <t>C[C@@H](CN1CCC(Cc2ccccc2)CC1)[C@@H](O)c3ccc(O)cc3</t>
+  </si>
+  <si>
+    <t>C17 H18 N3 O5 P</t>
+  </si>
+  <si>
+    <t>Oc1nc2cccc(C(NCCc3ccccc3)P(=O)(O)O)c2nc1O</t>
+  </si>
+  <si>
+    <t>C20H24ClNO3</t>
+  </si>
+  <si>
+    <t>COc1cc2CCN(C)[C@@H](C[C@H](O)c3ccc(Cl)cc3)c2cc1OC</t>
+  </si>
+  <si>
+    <t>C17H28Cl2N5O13P3S</t>
+  </si>
+  <si>
+    <t>CCCSc1nc(NCCOC)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C14H22F2N5O12P3S</t>
+  </si>
+  <si>
+    <t>CCCSc1nc(N)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(F)(F)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C13H20Cl2N5O12P3S</t>
+  </si>
+  <si>
+    <t>CCSc1nc(N)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C11H16Cl2N5O12P3</t>
+  </si>
+  <si>
+    <t>Nc1ncnc2c1ncn2[C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O</t>
+  </si>
+  <si>
+    <t>C17H25Cl2F3N5O12P3S2</t>
+  </si>
+  <si>
+    <t>CSCCNc1nc(SCCC(F)(F)F)nc2c1ncn2[C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O</t>
+  </si>
+  <si>
+    <t>C14H22Cl2N5O12P3S</t>
+  </si>
+  <si>
+    <t>CCCSc1nc(N)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C14H19Cl2F3N5O12P3S</t>
+  </si>
+  <si>
+    <t>Nc1nc(SCCC(F)(F)F)nc2c1ncn2[C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O</t>
+  </si>
+  <si>
+    <t>C22H27N5O2S</t>
+  </si>
+  <si>
+    <t>C[C@H](CN1CCN(CC1)C(=O)C)NC(=O)c2cc3c(nn(C)c3s2)c4ccccc4</t>
+  </si>
+  <si>
+    <t>C16H23Cl2F3N5O12P3S</t>
+  </si>
+  <si>
+    <t>CCCSc1nc(NCC(F)(F)F)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C24H30N6O2</t>
+  </si>
+  <si>
+    <t>CCCc1nc(oc1C(=O)NC(C)CN2CCN(CC2)c3ncccn3)c4ccccc4</t>
+  </si>
+  <si>
+    <t>C17H28Cl2N5O12P3S2</t>
+  </si>
+  <si>
+    <t>CCCSc1nc(NCCSC)c2ncn([C@@H]3O[C@H](COP(=O)(O)OP(=O)(O)C(Cl)(Cl)P(=O)(O)O)[C@@H](O)[C@H]3O)c2n1</t>
+  </si>
+  <si>
+    <t>C36 H34 O3</t>
+  </si>
+  <si>
+    <t>CCc1cc(ccc1c2cccc(Cc3ccc4ccccc4c3)c2)c5ccc(OCC(=O)O)cc5C(C)C</t>
+  </si>
+  <si>
+    <t>CCc1cc(ccc1c2cccc(Cc3cccc4ccccc34)c2)c5ccc(OCC(=O)O)cc5C(C)C</t>
+  </si>
+  <si>
+    <t>C19 H22 N4 O2</t>
+  </si>
+  <si>
+    <t>CCOc1ccccc1c2nc(O)n3c(C)nc(C4CCCC4)c3n2</t>
+  </si>
+  <si>
+    <t>C23 H31 N7 O5 S</t>
+  </si>
+  <si>
+    <t>CCOc1ccc(cc1c2nc(O)c3nnc(C4CCCC4)n3n2)S(=O)(=O)N5CCN(CCO)CC5</t>
+  </si>
+  <si>
+    <t>C15 H15 Br2 N5 O3 S</t>
+  </si>
+  <si>
+    <t>CCCCS(=O)(=O)Nc1cccc(c1)c2nnc(O)n3c(Br)c(Br)nc23</t>
+  </si>
+  <si>
+    <t>C24 H32 N6 O4 S</t>
+  </si>
+  <si>
+    <t>CCOc1ccc(cc1c2nc(O)c3c(C)nc(C4CCCC4)n3n2)S(=O)(=O)N5CCN(C)CC5</t>
+  </si>
+  <si>
+    <t>C25 H34 N6 O5 S</t>
+  </si>
+  <si>
+    <t>CCOc1ccc(cc1c2nc(O)c3c(C)nc(C4CCCC4)n3n2)S(=O)(=O)N5CCN(CCO)CC5</t>
+  </si>
+  <si>
+    <t>CCOc1ccc(cc1c2nc(O)n3c(C)nc(C4CCCC4)c3n2)S(=O)(=O)N5CCN(CCO)CC5</t>
+  </si>
+  <si>
+    <t>CCOc1ccc(cc1c2nc(O)c3c(n2)c(nn3C)C4CCCC4)S(=O)(=O)N5CCN(CCO)CC5</t>
+  </si>
+  <si>
+    <t>C25 H33 N3 O6</t>
+  </si>
+  <si>
+    <t>CCc1cc(C(=O)C)c(O)cc1OCc2cccc(n2)C(=O)NCCCCCCCC(=O)NO</t>
+  </si>
+  <si>
+    <t>CCOc1ccccc1c2nc(O)c3c(C)nc(C4CCCC4)n3n2</t>
+  </si>
+  <si>
+    <t>C29 H51 N O</t>
+  </si>
+  <si>
+    <t>CCN1C2C[C@H](C)C3C4CC[C@H](C(C)CCCC(C)C)[C@@]4(C)CCC3[C@@]2(C)CCC1=O</t>
+  </si>
+  <si>
+    <t>C33 H25 Cl2 N O5</t>
+  </si>
+  <si>
+    <t>Cc1c(C(=O)c2ccc3OC(Oc3c2)(c4ccc(Cl)cc4)c5ccc(Cl)cc5)c6ccccc6n1CCCC(=O)O</t>
+  </si>
+  <si>
+    <t>C15 H18 Cl N O</t>
+  </si>
+  <si>
+    <t>CN1[C@@H]2CCc3cc(Cl)ccc3[C@@]2(C)CCC1=O</t>
+  </si>
+  <si>
+    <t>C16 H17 N O</t>
+  </si>
+  <si>
+    <t>CC1=C2CCc3cc(C=C)ccc3N2CCC1=O</t>
+  </si>
+  <si>
+    <t>C25 H31 Cl N2 O2</t>
+  </si>
+  <si>
+    <t>C[C@]12CCC3C(CCC4NC(=O)C=C[C@]34C)C1CCC2C(=O)Nc5ccc(Cl)cc5</t>
+  </si>
+  <si>
+    <t>C26 H34 N2 O3</t>
+  </si>
+  <si>
+    <t>COc1ccccc1NC(=O)C2CCC3C4CCC5NC(=O)C=C[C@]5(C)C4CC[C@]23C</t>
+  </si>
+  <si>
+    <t>C25 H42 N2 O2</t>
+  </si>
+  <si>
+    <t>CCC(CC)N(C=O)[C@H]1CCC2C3CC[C@H]4N(C)C(=O)CC[C@]4(C)C3CC[C@]12C</t>
+  </si>
+  <si>
+    <t>C27 H46 N2 O2</t>
+  </si>
+  <si>
+    <t>CCCCCN([C@H]1CCC2C3CC[C@H]4N(C)C(=O)CC[C@]4(C)C3CC[C@]12C)C(=O)CC</t>
+  </si>
+  <si>
+    <t>C21 H20 Cl N O2</t>
+  </si>
+  <si>
+    <t>CC1=C2CCc3cc(OCc4ccc(Cl)cc4)ccc3N2CCC1=O</t>
+  </si>
+  <si>
+    <t>C19 H15 N O4</t>
+  </si>
+  <si>
+    <t>C=CCc1c(OC(=O)Nc2ccccc2)ccc3C=CC(=O)Oc13</t>
+  </si>
+  <si>
+    <t>C25 H33 N3 O2</t>
+  </si>
+  <si>
+    <t>C[C@]12CCC3C(CCC4NC(=O)C=C[C@]34C)C1CCC2C(=O)Nc5cccc(N)c5</t>
+  </si>
+  <si>
+    <t>C20 H25 N</t>
+  </si>
+  <si>
+    <t>CN(C)C[C@@H]1C2CCC(C2)[C@H]1c3ccc4ccccc4c3</t>
+  </si>
+  <si>
+    <t>C16 H20 I N O2</t>
+  </si>
+  <si>
+    <t>COC(=O)[C@@H]1C2CCC(C[C@H]1c3ccc(I)cc3)N2C</t>
+  </si>
+  <si>
+    <t>C16H16Cl2N2O</t>
+  </si>
+  <si>
+    <t>Clc1cccc(OC([C@H]2CCNC2)c3ccccn3)c1Cl</t>
+  </si>
+  <si>
+    <t>C18H19NOS</t>
+  </si>
+  <si>
+    <t>CNCC[C@H](Oc1cccc2ccccc12)c3cccs3</t>
+  </si>
+  <si>
+    <t>C23H24N2O2</t>
+  </si>
+  <si>
+    <t>C1CC(CCN1)C(Oc2ccccc2Oc3ccccc3)c4cccnc4</t>
+  </si>
+  <si>
+    <t>C19H24N2O</t>
+  </si>
+  <si>
+    <t>CCc1cccc(OC(C2CCNCC2)c3cccnc3)c1</t>
+  </si>
+  <si>
+    <t>C18H22N2OS</t>
+  </si>
+  <si>
+    <t>CSc1ccc(OC(C2CCNCC2)c3cccnc3)cc1</t>
+  </si>
+  <si>
+    <t>C17H18F2N2O</t>
+  </si>
+  <si>
+    <t>Fc1cccc(OC(C2CCNCC2)c3cccnc3)c1F</t>
+  </si>
+  <si>
+    <t>C17H18Cl2N2O</t>
+  </si>
+  <si>
+    <t>Clc1ccc(OC(C2CCNCC2)c3ccccn3)c(Cl)c1</t>
+  </si>
+  <si>
+    <t>C16H17F3N2O4S</t>
+  </si>
+  <si>
+    <t>CN(C)Cc1cc(ccc1Oc2ccc(OC(F)(F)F)cc2)S(=O)(=O)N</t>
+  </si>
+  <si>
+    <t>C28H27N5O2</t>
+  </si>
+  <si>
+    <t>CCn1c2ccccc2c3cc(CNc4cnc(cn4)c5ccc(C[C@H](N)C(=O)O)cc5)ccc13</t>
+  </si>
+  <si>
+    <t>C24H32N6O2</t>
+  </si>
+  <si>
+    <t>CC(Nc1nc(N)nc(n1)c2ccc(C[C@H](N)C(=O)O)cc2)C34CC5CC(CC(C5)C3)C4</t>
+  </si>
+  <si>
+    <t>C25H20F6N6O3</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1ccc(cc1)c2cc(OC(c3ccccc3n4ccc(n4)C(F)(F)F)C(F)(F)F)nc(N)n2)C(=O)O</t>
+  </si>
+  <si>
+    <t>C27H26N4O2</t>
+  </si>
+  <si>
+    <t>Cc1ccccc1c2ccccc2CNc3cnc(cn3)c4ccc(C[C@H](N)C(=O)O)cc4</t>
+  </si>
+  <si>
+    <t>C26H26N6O2</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)c2ccc(CNc3nc(N)nc(n3)c4ccc(C[C@H](N)C(=O)O)cc4)cc2</t>
+  </si>
+  <si>
+    <t>C25H24N6O2</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1ccc(cc1)c2nc(N)nc(NCc3ccc(cc3)c4ccccc4)n2)C(=O)O</t>
+  </si>
+  <si>
+    <t>CC(Nc1nc(N)nc(n1)c2ccc(C[C@H](N)C(=O)O)cc2)c3ccc(cc3)c4ccccc4</t>
+  </si>
+  <si>
+    <t>C25H25N5O2</t>
+  </si>
+  <si>
+    <t>C[C@@H](Nc1cc(nc(N)n1)c2ccc(C[C@H](N)C(=O)O)cc2)c3ccc4ccccc4c3</t>
+  </si>
+  <si>
+    <t>C24H22N4O2</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1ccc(cc1)c2cnc(NCc3ccc4ccccc4c3)cn2)C(=O)O</t>
+  </si>
+  <si>
+    <t>C25H26N6O2</t>
+  </si>
+  <si>
+    <t>CC(C)(Nc1nc(N)nc(n1)c2ccc(C[C@H](N)C(=O)O)cc2)c3ccc4ccccc4c3</t>
+  </si>
+  <si>
+    <t>C26H30N4O4</t>
+  </si>
+  <si>
+    <t>COc1ccc(CNc2cnc(cn2)c3ccc(C[C@H](N)C(=O)O)cc3)c(OC4CCCC4)c1</t>
   </si>
 </sst>
 </file>
@@ -2787,7 +3972,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2797,18 +3982,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="50"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="51"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFEC50A"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2930,21 +4103,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3302,7 +4472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D323"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3328,24 +4498,24 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>589</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>588</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -7830,8 +9000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G251"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7847,43 +9017,43 @@
         <v>585</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>358</v>
       </c>
       <c r="D3" t="s">
@@ -7900,13 +9070,13 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>363</v>
       </c>
       <c r="D4" t="s">
@@ -7923,13 +9093,13 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>368</v>
       </c>
       <c r="D5" t="s">
@@ -8870,1031 +10040,2877 @@
         <v>586</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="8" t="s">
         <v>0</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>912</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" t="s">
+        <v>915</v>
+      </c>
+      <c r="C48">
+        <v>343.42493000000002</v>
+      </c>
+      <c r="D48" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="s">
+        <v>917</v>
+      </c>
+      <c r="C49">
+        <v>417.35471000000001</v>
+      </c>
+      <c r="D49" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="s">
+        <v>919</v>
+      </c>
+      <c r="C50">
+        <v>432.55786999999998</v>
+      </c>
+      <c r="D50" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51" t="s">
+        <v>921</v>
+      </c>
+      <c r="C51">
+        <v>431.52346</v>
+      </c>
+      <c r="D51" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" t="s">
+        <v>923</v>
+      </c>
+      <c r="C52">
+        <v>447.49322000000001</v>
+      </c>
+      <c r="D52" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" t="s">
+        <v>925</v>
+      </c>
+      <c r="C53">
+        <v>210.20493999999999</v>
+      </c>
+      <c r="D53" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" t="s">
+        <v>927</v>
+      </c>
+      <c r="C54">
+        <v>469.52026000000001</v>
+      </c>
+      <c r="D54" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" t="s">
+        <v>929</v>
+      </c>
+      <c r="C55">
+        <v>190.1986</v>
+      </c>
+      <c r="D55" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56" t="s">
+        <v>931</v>
+      </c>
+      <c r="C56">
+        <v>368.88308000000001</v>
+      </c>
+      <c r="D56" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57" t="s">
+        <v>933</v>
+      </c>
+      <c r="C57">
+        <v>296.36689999999999</v>
+      </c>
+      <c r="D57" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" t="s">
+        <v>935</v>
+      </c>
+      <c r="C58">
+        <v>449.53876000000002</v>
+      </c>
+      <c r="D58" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59" t="s">
+        <v>937</v>
+      </c>
+      <c r="C59">
+        <v>472.62502999999998</v>
+      </c>
+      <c r="D59" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60" t="s">
+        <v>939</v>
+      </c>
+      <c r="C60">
+        <v>450.61950999999999</v>
+      </c>
+      <c r="D60" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61" t="s">
+        <v>941</v>
+      </c>
+      <c r="C61">
+        <v>458.59845000000001</v>
+      </c>
+      <c r="D61" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62" t="s">
+        <v>943</v>
+      </c>
+      <c r="C62">
+        <v>399.53125999999997</v>
+      </c>
+      <c r="D62" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63" t="s">
+        <v>945</v>
+      </c>
+      <c r="C63">
+        <v>460.59440999999998</v>
+      </c>
+      <c r="D63" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" t="s">
+        <v>947</v>
+      </c>
+      <c r="C64">
+        <v>324.42336</v>
+      </c>
+      <c r="D64" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65" t="s">
+        <v>947</v>
+      </c>
+      <c r="C65">
+        <v>324.42335000000003</v>
+      </c>
+      <c r="D65" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" t="s">
+        <v>950</v>
+      </c>
+      <c r="C66">
+        <v>280.36419999999998</v>
+      </c>
+      <c r="D66" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" t="s">
+        <v>952</v>
+      </c>
+      <c r="C67">
+        <v>521.67749000000003</v>
+      </c>
+      <c r="D67" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68" t="s">
+        <v>954</v>
+      </c>
+      <c r="C68">
+        <v>330.46769999999998</v>
+      </c>
+      <c r="D68" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" t="s">
+        <v>956</v>
+      </c>
+      <c r="C69">
+        <v>320.40499999999997</v>
+      </c>
+      <c r="D69" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" t="s">
+        <v>958</v>
+      </c>
+      <c r="C70">
+        <v>606.80014000000006</v>
+      </c>
+      <c r="D70" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71" t="s">
+        <v>960</v>
+      </c>
+      <c r="C71">
+        <v>319.39539000000002</v>
+      </c>
+      <c r="D71" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" t="s">
+        <v>962</v>
+      </c>
+      <c r="C72">
+        <v>275.36928</v>
+      </c>
+      <c r="D72" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" t="s">
+        <v>925</v>
+      </c>
+      <c r="C73">
+        <v>210.20493999999999</v>
+      </c>
+      <c r="D73" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74" t="s">
+        <v>965</v>
+      </c>
+      <c r="C74">
+        <v>206.19800000000001</v>
+      </c>
+      <c r="D74" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75" t="s">
+        <v>925</v>
+      </c>
+      <c r="C75">
+        <v>210.20493999999999</v>
+      </c>
+      <c r="D75" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76" t="s">
+        <v>968</v>
+      </c>
+      <c r="C76">
+        <v>513.50175000000002</v>
+      </c>
+      <c r="D76" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77" t="s">
+        <v>970</v>
+      </c>
+      <c r="C77">
+        <v>486.69137999999998</v>
+      </c>
+      <c r="D77" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78" t="s">
+        <v>968</v>
+      </c>
+      <c r="C78">
+        <v>513.50175000000002</v>
+      </c>
+      <c r="D78" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79" t="s">
+        <v>973</v>
+      </c>
+      <c r="C79">
+        <v>485.44859000000002</v>
+      </c>
+      <c r="D79" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" t="s">
+        <v>975</v>
+      </c>
+      <c r="C80">
+        <v>465.03010999999998</v>
+      </c>
+      <c r="D80" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" t="s">
+        <v>977</v>
+      </c>
+      <c r="C81">
+        <v>514.48981000000003</v>
+      </c>
+      <c r="D81" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82" t="s">
+        <v>979</v>
+      </c>
+      <c r="C82">
+        <v>434.54894000000002</v>
+      </c>
+      <c r="D82" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83" t="s">
+        <v>981</v>
+      </c>
+      <c r="C83">
+        <v>518.83389999999997</v>
+      </c>
+      <c r="D83" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84" t="s">
+        <v>983</v>
+      </c>
+      <c r="C84">
+        <v>319.39211999999998</v>
+      </c>
+      <c r="D84" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85" t="s">
+        <v>985</v>
+      </c>
+      <c r="C85">
+        <v>376.49462</v>
+      </c>
+      <c r="D85" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86" t="s">
+        <v>987</v>
+      </c>
+      <c r="C86">
+        <v>395.49619999999999</v>
+      </c>
+      <c r="D86" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87" t="s">
+        <v>989</v>
+      </c>
+      <c r="C87">
+        <v>309.40541000000002</v>
+      </c>
+      <c r="D87" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88" t="s">
+        <v>991</v>
+      </c>
+      <c r="C88">
+        <v>654.59450000000004</v>
+      </c>
+      <c r="D88" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89" t="s">
+        <v>993</v>
+      </c>
+      <c r="C89">
+        <v>401.95274999999998</v>
+      </c>
+      <c r="D89" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90" t="s">
+        <v>995</v>
+      </c>
+      <c r="C90">
+        <v>379.47044</v>
+      </c>
+      <c r="D90" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91" t="s">
+        <v>997</v>
+      </c>
+      <c r="C91">
+        <v>321.15471000000002</v>
+      </c>
+      <c r="D91" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92" t="s">
+        <v>999</v>
+      </c>
+      <c r="C92">
+        <v>348.46458999999999</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C93">
+        <v>270.33292</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C94">
+        <v>270.33292</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C95">
+        <v>457.50963999999999</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C96">
+        <v>505.71454999999997</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C97">
+        <v>575.59272999999996</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98" t="s">
+        <v>917</v>
+      </c>
+      <c r="C98">
+        <v>417.35471000000001</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C99">
+        <v>301.40654999999998</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C100">
+        <v>360.42734000000002</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C101">
+        <v>442.55599999999998</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C102">
+        <v>365.49180999999999</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C103">
+        <v>289.76002999999997</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C104">
+        <v>330.37169999999998</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C105">
+        <v>627.83747000000005</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C106">
+        <v>373.45092</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C107">
+        <v>586.76567</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C108">
+        <v>264.3648</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C109">
+        <v>261.34269999999998</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C110">
+        <v>255.31497999999999</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C111">
+        <v>269.34485999999998</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C112">
+        <v>340.84500000000003</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C113">
+        <v>355.47386</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C114">
+        <v>313.77989000000002</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C115">
+        <v>452.03311000000002</v>
+      </c>
+      <c r="D115" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C116">
+        <v>300.78113000000002</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C117">
+        <v>437.96346999999997</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C118">
+        <v>350.47892999999999</v>
+      </c>
+      <c r="D118" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C119">
+        <v>336.45236</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C120">
+        <v>295.40044</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C121">
+        <v>378.48728</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C122">
+        <v>437.47847999999999</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C123">
+        <v>466.33582999999999</v>
+      </c>
+      <c r="D123" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C124">
+        <v>440.94574</v>
+      </c>
+      <c r="D124" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C125">
+        <v>390.88706000000002</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C126">
+        <v>420.52724999999998</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C127">
+        <v>434.51078000000001</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C128">
+        <v>495.61531000000002</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C129">
+        <v>513.60577999999998</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C130">
+        <v>527.63235999999995</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C131">
+        <v>497.58812999999998</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C132">
+        <v>315.43313000000001</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C133">
+        <v>588.44050000000004</v>
+      </c>
+      <c r="D133" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C134">
+        <v>295.37884000000003</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C135">
+        <v>373.44761</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C136">
+        <v>308.41735999999997</v>
+      </c>
+      <c r="D136" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C137">
+        <v>222.28505999999999</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C138">
+        <v>580.43996000000004</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C139">
+        <v>375.42043000000001</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C140">
+        <v>373.44761</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C141">
+        <v>406.47422999999998</v>
+      </c>
+      <c r="D141" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C142">
+        <v>917.12789999999995</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="B143" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C143">
+        <v>277.40332000000001</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C144">
+        <v>222.28505999999999</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C145">
+        <v>354.44274000000001</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C146">
+        <v>437.52154000000002</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C147">
+        <v>451.59766999999999</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C148">
+        <v>354.48248999999998</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="B149" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C149">
+        <v>354.48248999999998</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C150">
+        <v>352.50967000000003</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="B151" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C151">
+        <v>338.48309999999998</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="B152" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C152">
+        <v>258.22949999999997</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="B153" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C153">
+        <v>255.26862</v>
+      </c>
+      <c r="D153" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="B154" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C154">
+        <v>354.48248999999998</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="B155" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C155">
+        <v>338.44002999999998</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="B156" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C156">
+        <v>324.45652000000001</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="B157" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C157">
+        <v>395.53440999999998</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="B158" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C158">
+        <v>321.38808</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="B159" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C159">
+        <v>257.35399999999998</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="B160" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C160">
+        <v>188.17940999999999</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C161">
+        <v>330.40472</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C162">
+        <v>442.50963000000002</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C163">
+        <v>472.33661000000001</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C164">
+        <v>267.07547</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="B165" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C165">
+        <v>340.37310000000002</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C166">
+        <v>326.34321</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C167">
+        <v>331.16073999999998</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="B168" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C168">
+        <v>315.43313000000001</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="B169" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C169">
+        <v>354.39636999999999</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="B170" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C170">
+        <v>337.3956</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="B171" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C171">
+        <v>283.25389999999999</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="B172" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C172">
+        <v>340.27069</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C173">
+        <v>276.26456000000002</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="B174" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C174">
+        <v>321.33</v>
+      </c>
+      <c r="D174" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C175">
+        <v>171.23831999999999</v>
+      </c>
+      <c r="D175" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="177" spans="1:1">
+      <c r="B176" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C176">
+        <v>366.36081999999999</v>
+      </c>
+      <c r="D176" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="178" spans="1:1">
+      <c r="B177" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C177">
+        <v>286.33231999999998</v>
+      </c>
+      <c r="D177" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="179" spans="1:1">
+      <c r="B178" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C178">
+        <v>287.31707</v>
+      </c>
+      <c r="D178" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="180" spans="1:1">
+      <c r="B179" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C179">
+        <v>312.36959999999999</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="181" spans="1:1">
+      <c r="B180" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C180">
+        <v>342.39558</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="182" spans="1:1">
+      <c r="B181" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C181">
+        <v>376.40368000000001</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="183" spans="1:1">
+      <c r="B182" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C182">
+        <v>353.39499999999998</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="184" spans="1:1">
+      <c r="B183" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C183">
+        <v>454.49887000000001</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="185" spans="1:1">
+      <c r="B184" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C184">
+        <v>503.52643</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="186" spans="1:1">
+      <c r="B185" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C185">
+        <v>466.53102999999999</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="187" spans="1:1">
+      <c r="B186" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C186">
+        <v>292.37819999999999</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="188" spans="1:1">
+      <c r="B187" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C187">
+        <v>218.20869999999999</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="189" spans="1:1">
+      <c r="B188" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C188">
+        <v>255.61464000000001</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="190" spans="1:1">
+      <c r="B189" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C189">
+        <v>334.41158000000001</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="191" spans="1:1">
+      <c r="B190" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C190">
+        <v>2093.21153</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="192" spans="1:1">
+      <c r="B191" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C191">
+        <v>316.06502999999998</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="193" spans="1:1">
+      <c r="B192" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C192">
+        <v>350.41098</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
       <c r="A193" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="194" spans="1:1">
+      <c r="B193" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C193">
+        <v>269.64121999999998</v>
+      </c>
+      <c r="D193" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
       <c r="A194" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="195" spans="1:1">
+      <c r="B194" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C194">
+        <v>407.46230000000003</v>
+      </c>
+      <c r="D194" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
       <c r="A195" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="196" spans="1:1">
+      <c r="B195" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C195">
+        <v>339.47116</v>
+      </c>
+      <c r="D195" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
       <c r="A196" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="197" spans="1:1">
+      <c r="B196" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C196">
+        <v>375.31567999999999</v>
+      </c>
+      <c r="D196" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
       <c r="A197" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="198" spans="1:1">
+      <c r="B197" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C197">
+        <v>361.86246</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
       <c r="A198" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="199" spans="1:1">
+      <c r="B198" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C198">
+        <v>706.32219999999995</v>
+      </c>
+      <c r="D198" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
       <c r="A199" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="200" spans="1:1">
+      <c r="B199" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C199">
+        <v>615.33385999999996</v>
+      </c>
+      <c r="D199" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
       <c r="A200" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="201" spans="1:1">
+      <c r="B200" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C200">
+        <v>634.21648000000005</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
       <c r="A201" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="202" spans="1:1">
+      <c r="B201" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C201">
+        <v>574.09831999999994</v>
+      </c>
+      <c r="D201" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
       <c r="A202" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="203" spans="1:1">
+      <c r="B202" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C202">
+        <v>776.35919000000001</v>
+      </c>
+      <c r="D202" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
       <c r="A203" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="204" spans="1:1">
+      <c r="B203" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C203">
+        <v>648.24306000000001</v>
+      </c>
+      <c r="D203" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
       <c r="A204" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="205" spans="1:1">
+      <c r="B204" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C204">
+        <v>702.21445000000006</v>
+      </c>
+      <c r="D204" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
       <c r="A205" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="206" spans="1:1">
+      <c r="B205" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C205">
+        <v>425.54707999999999</v>
+      </c>
+      <c r="D205" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
       <c r="A206" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="207" spans="1:1">
+      <c r="B206" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C206">
+        <v>730.26760999999999</v>
+      </c>
+      <c r="D206" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
       <c r="A207" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="208" spans="1:1">
+      <c r="B207" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C207">
+        <v>434.53399999999999</v>
+      </c>
+      <c r="D207" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
       <c r="A208" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="209" spans="1:1">
+      <c r="B208" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C208">
+        <v>722.38779999999997</v>
+      </c>
+      <c r="D208" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
       <c r="A209" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="210" spans="1:1">
+      <c r="B209" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C209">
+        <v>514.65335000000005</v>
+      </c>
+      <c r="D209" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
       <c r="A210" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="211" spans="1:1">
+      <c r="B210" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C210">
+        <v>514.65335000000005</v>
+      </c>
+      <c r="D210" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
       <c r="A211" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="212" spans="1:1">
+      <c r="B211" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C211">
+        <v>338.40357</v>
+      </c>
+      <c r="D211" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
       <c r="A212" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="213" spans="1:1">
+      <c r="B212" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C212">
+        <v>517.60113000000001</v>
+      </c>
+      <c r="D212" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
       <c r="A213" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="214" spans="1:1">
+      <c r="B213" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C213">
+        <v>505.18428999999998</v>
+      </c>
+      <c r="D213" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
       <c r="A214" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="215" spans="1:1">
+      <c r="B214" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C214">
+        <v>500.61367000000001</v>
+      </c>
+      <c r="D214" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
       <c r="A215" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="216" spans="1:1">
+      <c r="B215" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C215">
+        <v>530.63964999999996</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
       <c r="A216" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="217" spans="1:1">
+      <c r="B216" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C216">
+        <v>530.63964999999996</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
       <c r="A217" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="218" spans="1:1">
+      <c r="B217" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C217">
+        <v>530.63964999999996</v>
+      </c>
+      <c r="D217" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
       <c r="A218" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="219" spans="1:1">
+      <c r="B218" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C218">
+        <v>471.54601000000002</v>
+      </c>
+      <c r="D218" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
       <c r="A219" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="220" spans="1:1">
+      <c r="B219" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C219">
+        <v>338.40357</v>
+      </c>
+      <c r="D219" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
       <c r="A220" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="221" spans="1:1">
+      <c r="B220" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C220">
+        <v>429.72133000000002</v>
+      </c>
+      <c r="D220" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
       <c r="A221" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="222" spans="1:1">
+      <c r="B221" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C221">
+        <v>586.46130000000005</v>
+      </c>
+      <c r="D221" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
       <c r="A222" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="223" spans="1:1">
+      <c r="B222" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C222">
+        <v>263.76251999999999</v>
+      </c>
+      <c r="D222" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
       <c r="A223" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="224" spans="1:1">
+      <c r="B223" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C223">
+        <v>239.31227999999999</v>
+      </c>
+      <c r="D223" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
       <c r="A224" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="225" spans="1:1">
+      <c r="B224" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C224">
+        <v>426.97883999999999</v>
+      </c>
+      <c r="D224" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
       <c r="A225" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="226" spans="1:1">
+      <c r="B225" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C225">
+        <v>422.55975999999998</v>
+      </c>
+      <c r="D225" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
       <c r="A226" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="227" spans="1:1">
+      <c r="B226" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C226">
+        <v>402.61318</v>
+      </c>
+      <c r="D226" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
       <c r="A227" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="228" spans="1:1">
+      <c r="B227" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C227">
+        <v>430.66633000000002</v>
+      </c>
+      <c r="D227" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
       <c r="A228" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="229" spans="1:1">
+      <c r="B228" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C228">
+        <v>353.84199999999998</v>
+      </c>
+      <c r="D228" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
       <c r="A229" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="230" spans="1:1">
+      <c r="B229" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C229">
+        <v>321.32670000000002</v>
+      </c>
+      <c r="D229" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
       <c r="A230" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="231" spans="1:1">
+      <c r="B230" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C230">
+        <v>407.54842000000002</v>
+      </c>
+      <c r="D230" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
       <c r="A231" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="232" spans="1:1">
+      <c r="B231" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C231">
+        <v>279.41919999999999</v>
+      </c>
+      <c r="D231" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
       <c r="A232" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="233" spans="1:1">
+      <c r="B232" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C232">
+        <v>385.23997000000003</v>
+      </c>
+      <c r="D232" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
       <c r="A233" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="234" spans="1:1">
+      <c r="B233" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C233">
+        <v>323.21704</v>
+      </c>
+      <c r="D233" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
       <c r="A234" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="235" spans="1:1">
+      <c r="B234" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C234">
+        <v>297.41455999999999</v>
+      </c>
+      <c r="D234" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
       <c r="A235" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="236" spans="1:1">
+      <c r="B235" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C235">
+        <v>360.44886000000002</v>
+      </c>
+      <c r="D235" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
       <c r="A236" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="237" spans="1:1">
+      <c r="B236" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C236">
+        <v>296.40665999999999</v>
+      </c>
+      <c r="D236" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
       <c r="A237" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="238" spans="1:1">
+      <c r="B237" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C237">
+        <v>314.44508000000002</v>
+      </c>
+      <c r="D237" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
       <c r="A238" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="239" spans="1:1">
+      <c r="B238" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C238">
+        <v>304.33442000000002</v>
+      </c>
+      <c r="D238" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
       <c r="A239" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="240" spans="1:1">
+      <c r="B239" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C239">
+        <v>337.24362000000002</v>
+      </c>
+      <c r="D239" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
       <c r="A240" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="241" spans="1:1">
+      <c r="B240" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C240">
+        <v>390.37738000000002</v>
+      </c>
+      <c r="D240" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
       <c r="A241" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="242" spans="1:1">
+      <c r="B241" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C241">
+        <v>465.54628000000002</v>
+      </c>
+      <c r="D241" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
       <c r="A242" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="243" spans="1:1">
+      <c r="B242" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C242">
+        <v>436.54987999999997</v>
+      </c>
+      <c r="D242" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
       <c r="A243" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="244" spans="1:1">
+      <c r="B243" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C243">
+        <v>566.45510999999999</v>
+      </c>
+      <c r="D243" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
       <c r="A244" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="245" spans="1:1">
+      <c r="B244" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C244">
+        <v>438.52093000000002</v>
+      </c>
+      <c r="D244" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
       <c r="A245" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="246" spans="1:1">
+      <c r="B245" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C245">
+        <v>454.52363000000003</v>
+      </c>
+      <c r="D245" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
       <c r="A246" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="247" spans="1:1">
+      <c r="B246" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C246">
+        <v>440.49705999999998</v>
+      </c>
+      <c r="D246" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
       <c r="A247" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="248" spans="1:1">
+      <c r="B247" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C247">
+        <v>454.52364</v>
+      </c>
+      <c r="D247" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
       <c r="A248" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="249" spans="1:1">
+      <c r="B248" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C248">
+        <v>427.49829999999997</v>
+      </c>
+      <c r="D248" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
       <c r="A249" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="250" spans="1:1">
+      <c r="B249" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C249">
+        <v>398.45708000000002</v>
+      </c>
+      <c r="D249" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
       <c r="A250" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="251" spans="1:1">
+      <c r="B250" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C250">
+        <v>442.51292999999998</v>
+      </c>
+      <c r="D250" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
       <c r="A251" t="s">
         <v>351</v>
+      </c>
+      <c r="B251" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C251">
+        <v>462.54079000000002</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>